<commit_message>
Adding More Art Assets
Adding bunch of backgrounds, also the original files as well.
</commit_message>
<xml_diff>
--- a/_Important Documents/Asset List.xlsx
+++ b/_Important Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
   <si>
     <t>File Name</t>
   </si>
@@ -138,9 +138,6 @@
     <t>ms-menu</t>
   </si>
   <si>
-    <t>720 x 420 px</t>
-  </si>
-  <si>
     <t>720 x 720 px</t>
   </si>
   <si>
@@ -207,12 +204,6 @@
     <t>therapist background</t>
   </si>
   <si>
-    <t>bg-room</t>
-  </si>
-  <si>
-    <t>example room image for tests</t>
-  </si>
-  <si>
     <t>Cheremisinov.mp3</t>
   </si>
   <si>
@@ -223,6 +214,9 @@
   </si>
   <si>
     <t>final</t>
+  </si>
+  <si>
+    <t>420 x 720 px</t>
   </si>
 </sst>
 </file>
@@ -341,7 +335,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,7 +370,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,13 +622,13 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
@@ -648,7 +642,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -668,7 +662,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -688,7 +682,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -708,7 +702,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -728,7 +722,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -748,7 +742,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -768,7 +762,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -788,7 +782,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -808,7 +802,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -828,7 +822,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -848,7 +842,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -868,7 +862,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -888,7 +882,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -902,19 +896,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
-        <v>35</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -922,19 +916,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
         <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
@@ -942,13 +936,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -962,19 +956,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
         <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
       </c>
       <c r="F20" t="s">
         <v>35</v>
@@ -982,13 +976,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -1002,19 +996,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
         <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" t="s">
-        <v>35</v>
       </c>
       <c r="F22" t="s">
         <v>35</v>
@@ -1022,13 +1016,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -1042,47 +1036,47 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
         <v>43</v>
@@ -1091,10 +1085,10 @@
         <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
         <v>35</v>
@@ -1102,19 +1096,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F28" t="s">
         <v>35</v>
@@ -1122,44 +1116,24 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" t="s">
-        <v>41</v>
+        <v>62</v>
+      </c>
+      <c r="C29" s="2">
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="D29" t="s">
         <v>34</v>
       </c>
-      <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>66</v>
+      <c r="E29" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E30" r:id="rId1"/>
+    <hyperlink ref="E29" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
More work on gender, and fluidity.
</commit_message>
<xml_diff>
--- a/_Important Documents/Asset List.xlsx
+++ b/_Important Documents/Asset List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="19700" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t>File Name</t>
   </si>
@@ -204,12 +204,6 @@
     <t>therapist background</t>
   </si>
   <si>
-    <t>Cheremisinov.mp3</t>
-  </si>
-  <si>
-    <t>background  (Cheremisinov's Black Planet)</t>
-  </si>
-  <si>
     <t>http://freemusicarchive.org/music/Sergey_Cheremisinov/Dream/</t>
   </si>
   <si>
@@ -235,13 +229,55 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/1/1b/19th_century_Victorian_living_room,_Auckland_-_0816.jpg</t>
+  </si>
+  <si>
+    <t>Sergey Cheremisinov's Morning City</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Borrowed</t>
+  </si>
+  <si>
+    <t>music1.mp3</t>
+  </si>
+  <si>
+    <t>music2.mp3</t>
+  </si>
+  <si>
+    <t>music3.mp3</t>
+  </si>
+  <si>
+    <t>music4.mp3</t>
+  </si>
+  <si>
+    <t>music5.mps</t>
+  </si>
+  <si>
+    <t>music6.mps</t>
+  </si>
+  <si>
+    <t>Sergey Cheremisinov's Moonlight</t>
+  </si>
+  <si>
+    <t>Sergey Cheremisinov's Destroyer</t>
+  </si>
+  <si>
+    <t>Sergey Cheremisinov's Black Planet</t>
+  </si>
+  <si>
+    <t>Sergey Cheremisinov's Search and Fight</t>
+  </si>
+  <si>
+    <t>Sergey Cheremisinov's Escape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +289,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,9 +325,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -293,7 +338,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -353,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,22 +643,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="95" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -640,10 +686,10 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
@@ -652,7 +698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -660,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -672,7 +718,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -680,7 +726,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -692,7 +738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -700,7 +746,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -712,7 +758,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -720,7 +766,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -732,7 +778,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -740,7 +786,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -752,7 +798,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -760,7 +806,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -772,7 +818,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -780,7 +826,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -792,7 +838,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -800,7 +846,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -812,7 +858,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -820,7 +866,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -832,7 +878,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -840,7 +886,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -852,7 +898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -860,7 +906,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -872,7 +918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -880,7 +926,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -892,7 +938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -900,7 +946,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -912,7 +958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -923,7 +969,7 @@
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
@@ -932,7 +978,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -943,7 +989,7 @@
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -952,7 +998,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -963,16 +1009,16 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -983,7 +1029,7 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
@@ -992,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1003,16 +1049,16 @@
         <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" t="s">
         <v>68</v>
       </c>
-      <c r="F21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1023,7 +1069,7 @@
         <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
@@ -1032,7 +1078,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1043,16 +1089,16 @@
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1063,16 +1109,16 @@
         <v>40</v>
       </c>
       <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" t="s">
         <v>67</v>
       </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1083,7 +1129,7 @@
         <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
         <v>41</v>
@@ -1092,7 +1138,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1103,7 +1149,7 @@
         <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1112,7 +1158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1132,31 +1178,133 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6">
+      <c r="C29" s="2"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="2">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="2">
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>63</v>
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="2">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F29" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding More Character Assets
Adding character assets for officer 2 and old neighbour (peggy).
</commit_message>
<xml_diff>
--- a/_Important Documents/Asset List.xlsx
+++ b/_Important Documents/Asset List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="19700" windowHeight="16140"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19695" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,20 +645,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
     <col min="6" max="6" width="95" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -709,16 +709,16 @@
         <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -738,7 +738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -758,7 +758,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -769,16 +769,16 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -798,7 +798,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -818,7 +818,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -838,7 +838,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -858,7 +858,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -869,16 +869,16 @@
         <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -898,7 +898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -918,7 +918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -938,7 +938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -958,7 +958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -978,7 +978,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -998,7 +998,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1178,11 +1178,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
All Assets Are In Place
Added the remaining assets.
</commit_message>
<xml_diff>
--- a/_Important Documents/Asset List.xlsx
+++ b/_Important Documents/Asset List.xlsx
@@ -614,7 +614,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,10 +777,10 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -817,10 +817,10 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -837,10 +837,10 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Final Asset List Added
Added original image references to the Asset List.
</commit_message>
<xml_diff>
--- a/_Important Documents/Asset List.xlsx
+++ b/_Important Documents/Asset List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="19700" windowHeight="16140"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19695" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
   <si>
     <t>File Name</t>
   </si>
@@ -120,9 +120,6 @@
     <t>http://cdn1.thr.com/sites/default/files/imagecache/675x380/2014/09/gotham_police_station_set_design.jpg</t>
   </si>
   <si>
-    <t>final-ish</t>
-  </si>
-  <si>
     <t>borrowed</t>
   </si>
   <si>
@@ -277,6 +274,45 @@
   </si>
   <si>
     <t>https://www.freesound.org/people/acclivity/sounds/24929/</t>
+  </si>
+  <si>
+    <t>edited</t>
+  </si>
+  <si>
+    <t>Edited from: bg-living.jpg</t>
+  </si>
+  <si>
+    <t>Edited from: bg-garden.jpg</t>
+  </si>
+  <si>
+    <t>Edited from: bg-therapist.jpg</t>
+  </si>
+  <si>
+    <t>Edited from: bg-station.jpg</t>
+  </si>
+  <si>
+    <t>bg-kitchen-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-dining-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-living-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-bath-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-garden-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-lake-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-station-original.jpg</t>
+  </si>
+  <si>
+    <t>bg-therapist-original.jpg</t>
   </si>
 </sst>
 </file>
@@ -649,22 +685,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
     <col min="6" max="6" width="95" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,9 +720,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -704,9 +740,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -724,9 +760,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -744,9 +780,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -764,9 +800,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -784,9 +820,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -804,9 +840,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -824,9 +860,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -844,9 +880,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -864,9 +900,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -884,9 +920,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -904,9 +940,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -924,9 +960,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -935,18 +971,18 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -964,9 +1000,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -975,18 +1011,18 @@
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
@@ -1004,9 +1040,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
@@ -1015,18 +1051,18 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -1035,280 +1071,440 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
         <v>33</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
         <v>34</v>
       </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="2">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="2">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="D40" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="2">
-        <v>9.5138888888888884E-2</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E40" t="s">
         <v>39</v>
       </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="F40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="2">
-        <v>7.0833333333333331E-2</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
         <v>39</v>
       </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="F41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" t="s">
         <v>39</v>
       </c>
-      <c r="E29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="F42" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" t="s">
         <v>39</v>
       </c>
-      <c r="E30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="2">
-        <v>6.7361111111111108E-2</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="F43" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" t="s">
         <v>39</v>
       </c>
-      <c r="E31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="2">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="D33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="F44" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C35" s="2">
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="D35" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F33" r:id="rId1"/>
-    <hyperlink ref="F34" r:id="rId2"/>
-    <hyperlink ref="F35" r:id="rId3"/>
+    <hyperlink ref="F42" r:id="rId1"/>
+    <hyperlink ref="F43" r:id="rId2"/>
+    <hyperlink ref="F44" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>